<commit_message>
Re-Arrange for PCB part
</commit_message>
<xml_diff>
--- a/schpcb/原理图及LayoutPCB设计规范.xlsx
+++ b/schpcb/原理图及LayoutPCB设计规范.xlsx
@@ -841,74 +841,74 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,7 +1294,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="23">
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1307,8 +1307,8 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1318,8 +1318,8 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="5" t="s">
         <v>0</v>
       </c>
@@ -1327,8 +1327,8 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1338,8 +1338,8 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="5" t="s">
         <v>96</v>
       </c>
@@ -1347,8 +1347,8 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1358,8 +1358,8 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
@@ -1367,8 +1367,8 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="30"/>
+      <c r="B14" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1378,8 +1378,8 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
@@ -1387,8 +1387,8 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1398,8 +1398,8 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1407,8 +1407,8 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1416,10 +1416,10 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
+      <c r="A19" s="23">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1429,8 +1429,8 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="6" t="s">
         <v>86</v>
       </c>
@@ -1438,7 +1438,7 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="12" t="s">
         <v>102</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="12" t="s">
         <v>103</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="12" t="s">
         <v>105</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="12" t="s">
         <v>107</v>
       </c>
@@ -1482,7 +1482,7 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="12" t="s">
         <v>114</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="12" t="s">
         <v>120</v>
       </c>
@@ -1504,7 +1504,7 @@
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="12" t="s">
         <v>135</v>
       </c>
@@ -1515,7 +1515,7 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="12" t="s">
         <v>122</v>
       </c>
@@ -1526,7 +1526,7 @@
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="12" t="s">
         <v>137</v>
       </c>
@@ -1537,7 +1537,7 @@
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="12" t="s">
         <v>124</v>
       </c>
@@ -1548,7 +1548,7 @@
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="12" t="s">
         <v>109</v>
       </c>
@@ -1559,7 +1559,7 @@
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="12" t="s">
         <v>126</v>
       </c>
@@ -1570,7 +1570,7 @@
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="12" t="s">
         <v>117</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="12" t="s">
         <v>112</v>
       </c>
@@ -1592,7 +1592,7 @@
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="12" t="s">
         <v>119</v>
       </c>
@@ -1603,10 +1603,10 @@
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="16">
+      <c r="A36" s="23">
         <v>6</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="27" t="s">
         <v>87</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -1616,8 +1616,8 @@
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="17"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="5" t="s">
         <v>32</v>
       </c>
@@ -1625,8 +1625,8 @@
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="15"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="5" t="s">
         <v>33</v>
       </c>
@@ -1634,7 +1634,7 @@
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="16">
+      <c r="A39" s="23">
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1645,8 +1645,8 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="17"/>
-      <c r="B40" s="13" t="s">
+      <c r="A40" s="30"/>
+      <c r="B40" s="27" t="s">
         <v>88</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -1656,8 +1656,8 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="14"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="5" t="s">
         <v>128</v>
       </c>
@@ -1665,8 +1665,8 @@
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="14"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="5" t="s">
         <v>129</v>
       </c>
@@ -1674,8 +1674,8 @@
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43" s="14"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="5" t="s">
         <v>130</v>
       </c>
@@ -1683,8 +1683,8 @@
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
-      <c r="B44" s="15"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="5" t="s">
         <v>75</v>
       </c>
@@ -1692,8 +1692,8 @@
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45" s="13" t="s">
+      <c r="A45" s="30"/>
+      <c r="B45" s="27" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -1703,8 +1703,8 @@
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
-      <c r="B46" s="14"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="5" t="s">
         <v>74</v>
       </c>
@@ -1712,8 +1712,8 @@
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
-      <c r="B47" s="14"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="5" t="s">
         <v>73</v>
       </c>
@@ -1721,8 +1721,8 @@
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="5" t="s">
         <v>72</v>
       </c>
@@ -1730,8 +1730,8 @@
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="17"/>
-      <c r="B49" s="13" t="s">
+      <c r="A49" s="30"/>
+      <c r="B49" s="27" t="s">
         <v>90</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1741,8 +1741,8 @@
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="5" t="s">
         <v>131</v>
       </c>
@@ -1750,8 +1750,8 @@
       <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="17"/>
-      <c r="B51" s="14"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="5" t="s">
         <v>132</v>
       </c>
@@ -1759,8 +1759,8 @@
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="17"/>
-      <c r="B52" s="14"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="5" t="s">
         <v>133</v>
       </c>
@@ -1768,8 +1768,8 @@
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="17"/>
-      <c r="B53" s="15"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="5" t="s">
         <v>134</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
         <v>91</v>
       </c>
@@ -1788,10 +1788,10 @@
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="16">
+      <c r="A55" s="23">
         <v>8</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="27" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -1801,8 +1801,8 @@
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56" s="14"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="5" t="s">
         <v>77</v>
       </c>
@@ -1810,8 +1810,8 @@
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="17"/>
-      <c r="B57" s="14"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="5" t="s">
         <v>29</v>
       </c>
@@ -1819,8 +1819,8 @@
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="17"/>
-      <c r="B58" s="14"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="5" t="s">
         <v>78</v>
       </c>
@@ -1828,8 +1828,8 @@
       <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="17"/>
-      <c r="B59" s="14"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="5" t="s">
         <v>30</v>
       </c>
@@ -1837,8 +1837,8 @@
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
-      <c r="B60" s="14"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="5" t="s">
         <v>26</v>
       </c>
@@ -1846,8 +1846,8 @@
       <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="18"/>
-      <c r="B61" s="15"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="5" t="s">
         <v>27</v>
       </c>
@@ -1881,10 +1881,10 @@
       <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A64" s="16">
+      <c r="A64" s="23">
         <v>11</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="22" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="11" t="s">
@@ -1894,8 +1894,8 @@
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A65" s="18"/>
-      <c r="B65" s="19"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="22"/>
       <c r="C65" s="6" t="s">
         <v>36</v>
       </c>
@@ -1904,6 +1904,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="A7:A18"/>
     <mergeCell ref="B64:B65"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B8:B9"/>
@@ -1920,8 +1922,6 @@
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="A7:A18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1933,15 +1933,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="25"/>
+    <col min="1" max="1" width="9" style="16"/>
     <col min="2" max="3" width="18.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="69" style="22" customWidth="1"/>
+    <col min="4" max="4" width="69" style="13" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
@@ -1954,16 +1954,16 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="20" t="s">
         <v>141</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="5" t="s">
         <v>139</v>
       </c>
@@ -1972,10 +1972,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="33">
+      <c r="A4" s="31">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1988,9 +1988,9 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="13" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="27" t="s">
         <v>144</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -2000,45 +2000,45 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="27" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="17" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="27" t="s">
+      <c r="A7" s="33"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="17" t="s">
         <v>66</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="33">
+      <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="18" t="s">
         <v>67</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="34"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="6" t="s">
         <v>145</v>
       </c>
@@ -2046,9 +2046,9 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="6" t="s">
         <v>69</v>
       </c>
@@ -2056,9 +2056,9 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="34"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="6" t="s">
         <v>68</v>
       </c>
@@ -2066,9 +2066,9 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="6" t="s">
         <v>70</v>
       </c>
@@ -2076,20 +2076,20 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="29" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="18" t="s">
         <v>168</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="5" t="s">
         <v>146</v>
       </c>
@@ -2098,8 +2098,8 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="5" t="s">
         <v>147</v>
       </c>
@@ -2108,20 +2108,20 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="5" t="s">
         <v>148</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="5" t="s">
         <v>150</v>
       </c>
@@ -2132,8 +2132,8 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="5" t="s">
         <v>152</v>
       </c>
@@ -2144,8 +2144,8 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="5" t="s">
         <v>153</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="33">
+      <c r="A20" s="31">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="27" t="s">
         <v>155</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -2172,8 +2172,8 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="5" t="s">
         <v>158</v>
       </c>
@@ -2184,8 +2184,8 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="5" t="s">
         <v>160</v>
       </c>
@@ -2196,31 +2196,31 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="34"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="31" t="s">
+      <c r="A23" s="32"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="35" t="s">
         <v>162</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="28" t="s">
+      <c r="A24" s="32"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="18" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="34"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="31"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="6" t="s">
         <v>51</v>
       </c>
@@ -2228,9 +2228,9 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="34"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="31"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="6" t="s">
         <v>52</v>
       </c>
@@ -2238,8 +2238,8 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="5" t="s">
         <v>48</v>
       </c>
@@ -2250,8 +2250,8 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
-      <c r="B28" s="14"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="5" t="s">
         <v>54</v>
       </c>
@@ -2262,8 +2262,8 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="5" t="s">
         <v>55</v>
       </c>
@@ -2274,8 +2274,8 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="5" t="s">
         <v>57</v>
       </c>
@@ -2286,8 +2286,8 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="5" t="s">
         <v>59</v>
       </c>
@@ -2298,9 +2298,9 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="29" t="s">
+      <c r="A32" s="33"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="19" t="s">
         <v>61</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -2310,10 +2310,10 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="33">
+      <c r="A33" s="31">
         <v>4</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="35" t="s">
         <v>164</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -2326,9 +2326,9 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="34"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32" t="s">
+      <c r="A34" s="32"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="21" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="6"/>
@@ -2336,9 +2336,9 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="34"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32" t="s">
+      <c r="A35" s="32"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="21" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="6"/>
@@ -2346,9 +2346,9 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="34"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="32" t="s">
+      <c r="A36" s="32"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="6"/>
@@ -2356,9 +2356,9 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="34"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="32" t="s">
+      <c r="A37" s="32"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="6"/>
@@ -2366,9 +2366,9 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="34"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="29" t="s">
+      <c r="A38" s="32"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="19" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="6"/>
@@ -2376,9 +2376,9 @@
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="34"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="29" t="s">
+      <c r="A39" s="32"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="6"/>
@@ -2386,9 +2386,9 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="34"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="29" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="6"/>
@@ -2396,9 +2396,9 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="34"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="29" t="s">
+      <c r="A41" s="32"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D41" s="6"/>
@@ -2406,9 +2406,9 @@
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="35"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="29" t="s">
+      <c r="A42" s="33"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="19" t="s">
         <v>62</v>
       </c>
       <c r="D42" s="6"/>
@@ -2416,7 +2416,7 @@
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:7" ht="33" x14ac:dyDescent="0.3">
-      <c r="A43" s="30">
+      <c r="A43" s="20">
         <v>5</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -2432,7 +2432,7 @@
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
@@ -2440,15 +2440,15 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="29"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
@@ -2461,75 +2461,75 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C48" s="4"/>
-      <c r="D48" s="24"/>
+      <c r="D48" s="15"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C49" s="4"/>
-      <c r="D49" s="24"/>
+      <c r="D49" s="15"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C50" s="4"/>
-      <c r="D50" s="24"/>
+      <c r="D50" s="15"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C51" s="4"/>
-      <c r="D51" s="24"/>
+      <c r="D51" s="15"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
-      <c r="D52" s="24"/>
+      <c r="D52" s="15"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C53" s="3"/>
-      <c r="D53" s="23"/>
+      <c r="D53" s="14"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C54" s="3"/>
-      <c r="D54" s="23"/>
+      <c r="D54" s="14"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C55" s="3"/>
-      <c r="D55" s="23"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C56" s="3"/>
-      <c r="D56" s="23"/>
+      <c r="D56" s="14"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D57" s="23"/>
+      <c r="D57" s="14"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D58" s="23"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -2537,13 +2537,13 @@
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="23"/>
+      <c r="D59" s="14"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D60" s="23"/>
+      <c r="D60" s="14"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -2551,7 +2551,7 @@
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="23"/>
+      <c r="D61" s="14"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -2559,7 +2559,7 @@
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="23"/>
+      <c r="D62" s="14"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -2567,7 +2567,7 @@
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="23"/>
+      <c r="D63" s="14"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -2575,7 +2575,7 @@
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="23"/>
+      <c r="D64" s="14"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>

</xml_diff>